<commit_message>
Still facing issues with GPIO3 being read in as 0 and counting in ULP
</commit_message>
<xml_diff>
--- a/ULP-Power.xlsx
+++ b/ULP-Power.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaidica/Documents/Arduino-ESP32/libraries/Hublink-BEAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D8A5C6-A954-5645-AB2D-77A4E2C20B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B221F506-1FC2-EC4D-AE50-3CD449899A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35300" yWindow="740" windowWidth="28040" windowHeight="17440" xr2:uid="{D7704C50-F320-E04F-98FC-86C01CBA9DF7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
   <si>
     <t>Name/Component</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>I2C held; removed RT9080 pull-down</t>
+  </si>
+  <si>
+    <t>Bare S3</t>
+  </si>
+  <si>
+    <t>BEAM Hublink</t>
+  </si>
+  <si>
+    <t>Presumably during GPIO interrupt?</t>
   </si>
 </sst>
 </file>
@@ -135,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +153,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5908D8F5-BBCB-4D42-A041-33E413097497}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,6 +704,69 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>150</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2">
+        <v>25</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>